<commit_message>
HTML encoding of string from and to with the given tag
</commit_message>
<xml_diff>
--- a/JS_Tracker.xlsx
+++ b/JS_Tracker.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
   <si>
     <t>Problem</t>
   </si>
@@ -329,6 +329,12 @@
   </si>
   <si>
     <t>JsonStringify</t>
+  </si>
+  <si>
+    <t>JsonParse</t>
+  </si>
+  <si>
+    <t>HTMLEncodingOfStr</t>
   </si>
 </sst>
 </file>
@@ -545,7 +551,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -625,6 +631,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -919,10 +926,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="C2:G77"/>
+  <dimension ref="C2:G79"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B61" workbookViewId="0">
-      <selection activeCell="E74" sqref="E74"/>
+      <selection activeCell="E77" sqref="E77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1465,6 +1472,18 @@
     <row r="77" spans="3:4">
       <c r="C77" s="2" t="s">
         <v>83</v>
+      </c>
+      <c r="D77" s="49"/>
+    </row>
+    <row r="78" spans="3:4">
+      <c r="C78" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D78" s="49"/>
+    </row>
+    <row r="79" spans="3:4">
+      <c r="C79" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
React class component lifecycle methods (mounting, updating, unmounting phase methods)
</commit_message>
<xml_diff>
--- a/JS_Tracker.xlsx
+++ b/JS_Tracker.xlsx
@@ -671,7 +671,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -755,6 +755,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1053,8 +1056,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="C2:G106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="E93" sqref="E93"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="D93" sqref="D93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1683,10 +1686,12 @@
       </c>
     </row>
     <row r="92" spans="3:6" ht="28.8">
-      <c r="C92" s="52" t="s">
+      <c r="C92" s="53" t="s">
         <v>98</v>
       </c>
-      <c r="F92" s="52" t="s">
+      <c r="D92" s="12"/>
+      <c r="E92" s="12"/>
+      <c r="F92" s="53" t="s">
         <v>99</v>
       </c>
     </row>

</xml_diff>